<commit_message>
add initial project stuff
</commit_message>
<xml_diff>
--- a/projects/EcoFoci/dy2012/data/dy2012_faire.xlsx
+++ b/projects/EcoFoci/dy2012/data/dy2012_faire.xlsx
@@ -5959,7 +5959,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>E26.2B.DY2012 | E26.1B.DY2012</t>
+          <t>E26.1B.DY2012 | E26.2B.DY2012</t>
         </is>
       </c>
       <c r="J5" t="n">
@@ -6649,7 +6649,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>E26.2B.DY2012 | E26.1B.DY2012</t>
+          <t>E26.1B.DY2012 | E26.2B.DY2012</t>
         </is>
       </c>
       <c r="J6" t="n">
@@ -7339,7 +7339,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>E27.2B.DY2012 | E27.1B.DY2012</t>
+          <t>E27.1B.DY2012 | E27.2B.DY2012</t>
         </is>
       </c>
       <c r="J7" t="n">
@@ -8031,7 +8031,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>E27.2B.DY2012 | E27.1B.DY2012</t>
+          <t>E27.1B.DY2012 | E27.2B.DY2012</t>
         </is>
       </c>
       <c r="J8" t="n">
@@ -8723,7 +8723,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>E28.2B.DY2012 | E28.1B.DY2012</t>
+          <t>E28.1B.DY2012 | E28.2B.DY2012</t>
         </is>
       </c>
       <c r="J9" t="n">
@@ -9413,7 +9413,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>E28.2B.DY2012 | E28.1B.DY2012</t>
+          <t>E28.1B.DY2012 | E28.2B.DY2012</t>
         </is>
       </c>
       <c r="J10" t="n">
@@ -11487,7 +11487,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>E30.1B.DY2012 | E30.2B.DY2012</t>
+          <t>E30.2B.DY2012 | E30.1B.DY2012</t>
         </is>
       </c>
       <c r="J13" t="n">
@@ -12177,7 +12177,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>E30.1B.DY2012 | E30.2B.DY2012</t>
+          <t>E30.2B.DY2012 | E30.1B.DY2012</t>
         </is>
       </c>
       <c r="J14" t="n">
@@ -22543,7 +22543,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>E38.2B.DY2012 | E38.1B.DY2012</t>
+          <t>E38.1B.DY2012 | E38.2B.DY2012</t>
         </is>
       </c>
       <c r="J29" t="n">
@@ -23233,7 +23233,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>E38.2B.DY2012 | E38.1B.DY2012</t>
+          <t>E38.1B.DY2012 | E38.2B.DY2012</t>
         </is>
       </c>
       <c r="J30" t="n">
@@ -25303,7 +25303,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>E40.1B.DY2012 | E40.2B.DY2012</t>
+          <t>E40.2B.DY2012 | E40.1B.DY2012</t>
         </is>
       </c>
       <c r="J33" t="n">
@@ -25995,7 +25995,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>E40.1B.DY2012 | E40.2B.DY2012</t>
+          <t>E40.2B.DY2012 | E40.1B.DY2012</t>
         </is>
       </c>
       <c r="J34" t="n">
@@ -26687,7 +26687,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>E42.2B.DY2012 | E42.1B.DY2012</t>
+          <t>E42.1B.DY2012 | E42.2B.DY2012</t>
         </is>
       </c>
       <c r="J35" t="n">
@@ -27379,7 +27379,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>E42.2B.DY2012 | E42.1B.DY2012</t>
+          <t>E42.1B.DY2012 | E42.2B.DY2012</t>
         </is>
       </c>
       <c r="J36" t="n">
@@ -30123,7 +30123,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>E45.2B.DY2012 | E45.1B.DY2012</t>
+          <t>E45.1B.DY2012 | E45.2B.DY2012</t>
         </is>
       </c>
       <c r="J40" t="n">
@@ -30813,7 +30813,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>E45.2B.DY2012 | E45.1B.DY2012</t>
+          <t>E45.1B.DY2012 | E45.2B.DY2012</t>
         </is>
       </c>
       <c r="J41" t="n">
@@ -31503,7 +31503,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>E46.1B.DY2012 | E46.2B.DY2012</t>
+          <t>E46.2B.DY2012 | E46.1B.DY2012</t>
         </is>
       </c>
       <c r="J42" t="n">
@@ -32195,7 +32195,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>E46.1B.DY2012 | E46.2B.DY2012</t>
+          <t>E46.2B.DY2012 | E46.1B.DY2012</t>
         </is>
       </c>
       <c r="J43" t="n">
@@ -35631,7 +35631,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>E49.1B.DY2012 | E49.2B.DY2012</t>
+          <t>E49.2B.DY2012 | E49.1B.DY2012</t>
         </is>
       </c>
       <c r="J48" t="n">
@@ -36321,7 +36321,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>E49.1B.DY2012 | E49.2B.DY2012</t>
+          <t>E49.2B.DY2012 | E49.1B.DY2012</t>
         </is>
       </c>
       <c r="J49" t="n">
@@ -38395,7 +38395,7 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>E51.1B.DY2012 | E51.2B.DY2012</t>
+          <t>E51.2B.DY2012 | E51.1B.DY2012</t>
         </is>
       </c>
       <c r="J52" t="n">
@@ -39085,7 +39085,7 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>E51.1B.DY2012 | E51.2B.DY2012</t>
+          <t>E51.2B.DY2012 | E51.1B.DY2012</t>
         </is>
       </c>
       <c r="J53" t="n">
@@ -39775,7 +39775,7 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>E52.1B.DY2012 | E52.2B.DY2012</t>
+          <t>E52.2B.DY2012 | E52.1B.DY2012</t>
         </is>
       </c>
       <c r="J54" t="n">
@@ -40467,7 +40467,7 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>E52.1B.DY2012 | E52.2B.DY2012</t>
+          <t>E52.2B.DY2012 | E52.1B.DY2012</t>
         </is>
       </c>
       <c r="J55" t="n">
@@ -43903,7 +43903,7 @@
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>E55.1B.DY2012 | E55.2B.DY2012</t>
+          <t>E55.2B.DY2012 | E55.1B.DY2012</t>
         </is>
       </c>
       <c r="J60" t="n">
@@ -44593,7 +44593,7 @@
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>E55.1B.DY2012 | E55.2B.DY2012</t>
+          <t>E55.2B.DY2012 | E55.1B.DY2012</t>
         </is>
       </c>
       <c r="J61" t="n">
@@ -50791,7 +50791,7 @@
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>E61.1B.DY2012 | E61.2B.DY2012</t>
+          <t>E61.2B.DY2012 | E61.1B.DY2012</t>
         </is>
       </c>
       <c r="J70" t="n">
@@ -51483,7 +51483,7 @@
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>E61.1B.DY2012 | E61.2B.DY2012</t>
+          <t>E61.2B.DY2012 | E61.1B.DY2012</t>
         </is>
       </c>
       <c r="J71" t="n">
@@ -53535,7 +53535,7 @@
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>E63.1B.DY2012 | E63.2B.DY2012</t>
+          <t>E63.2B.DY2012 | E63.1B.DY2012</t>
         </is>
       </c>
       <c r="J74" t="n">
@@ -54227,7 +54227,7 @@
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>E63.1B.DY2012 | E63.2B.DY2012</t>
+          <t>E63.2B.DY2012 | E63.1B.DY2012</t>
         </is>
       </c>
       <c r="J75" t="n">
@@ -56279,7 +56279,7 @@
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t>E65.1B.DY2012 | E65.2B.DY2012</t>
+          <t>E65.2B.DY2012 | E65.1B.DY2012</t>
         </is>
       </c>
       <c r="J78" t="n">
@@ -56971,7 +56971,7 @@
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>E65.1B.DY2012 | E65.2B.DY2012</t>
+          <t>E65.2B.DY2012 | E65.1B.DY2012</t>
         </is>
       </c>
       <c r="J79" t="n">
@@ -59023,7 +59023,7 @@
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>E67.2B.DY2012 | E67.1B.DY2012</t>
+          <t>E67.1B.DY2012 | E67.2B.DY2012</t>
         </is>
       </c>
       <c r="J82" t="n">
@@ -59715,7 +59715,7 @@
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>E67.2B.DY2012 | E67.1B.DY2012</t>
+          <t>E67.1B.DY2012 | E67.2B.DY2012</t>
         </is>
       </c>
       <c r="J83" t="n">
@@ -63171,7 +63171,7 @@
       </c>
       <c r="I88" t="inlineStr">
         <is>
-          <t>E70.2B.DY2012 | E70.1B.DY2012</t>
+          <t>E70.1B.DY2012 | E70.2B.DY2012</t>
         </is>
       </c>
       <c r="J88" t="n">
@@ -63861,7 +63861,7 @@
       </c>
       <c r="I89" t="inlineStr">
         <is>
-          <t>E70.2B.DY2012 | E70.1B.DY2012</t>
+          <t>E70.1B.DY2012 | E70.2B.DY2012</t>
         </is>
       </c>
       <c r="J89" t="n">
@@ -64551,7 +64551,7 @@
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>E71.1B.DY2012 | E71.2B.DY2012</t>
+          <t>E71.2B.DY2012 | E71.1B.DY2012</t>
         </is>
       </c>
       <c r="J90" t="n">
@@ -65243,7 +65243,7 @@
       </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>E71.1B.DY2012 | E71.2B.DY2012</t>
+          <t>E71.2B.DY2012 | E71.1B.DY2012</t>
         </is>
       </c>
       <c r="J91" t="n">

</xml_diff>